<commit_message>
added HY34 in rn20a
</commit_message>
<xml_diff>
--- a/data/05.local.xlsx
+++ b/data/05.local.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/orion/Library/Caches/Transmit/590175CC-3AC2-4A78-89EE-519DE9F95424/login.msi.umn.edu/panfs/roc/groups/15/springer/zhoux379/projects/barn/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/orion/Library/Caches/Transmit/22D28208-F609-440A-B67C-CF5B61D4FD92/login.msi.umn.edu/panfs/roc/groups/15/springer/zhoux379/projects/barn/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808BE549-90E9-4445-9BFA-39D8380B5803}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B6E5789-7635-D84A-A245-6E6DD35DB6E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19380" yWindow="4540" windowWidth="24260" windowHeight="19960" firstSheet="11" activeTab="16" xr2:uid="{BEECB516-7BE0-DE4B-A089-736158D65AE9}"/>
+    <workbookView xWindow="16760" yWindow="4420" windowWidth="24260" windowHeight="19960" firstSheet="11" activeTab="16" xr2:uid="{BEECB516-7BE0-DE4B-A089-736158D65AE9}"/>
   </bookViews>
   <sheets>
     <sheet name="sp014" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11104" uniqueCount="4592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11107" uniqueCount="4594">
   <si>
     <t>SampleID</t>
   </si>
@@ -13827,6 +13827,12 @@
   </si>
   <si>
     <t>NM9</t>
+  </si>
+  <si>
+    <t>/home/springer/data_release/umgc/novaseq/200226_A00223_0330_BH2WT2DSXY/Springer_Project_069</t>
+  </si>
+  <si>
+    <t>HY34_S88</t>
   </si>
 </sst>
 </file>
@@ -20936,10 +20942,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26A2E0E7-B24A-E545-A8AB-EE5C932ADD80}">
-  <dimension ref="A1:G291"/>
+  <dimension ref="A1:G292"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55:XFD55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G292" sqref="G292"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23288,6 +23294,17 @@
       </c>
       <c r="G291" t="s">
         <v>4492</v>
+      </c>
+    </row>
+    <row r="292" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A292" t="s">
+        <v>3535</v>
+      </c>
+      <c r="F292" t="s">
+        <v>4592</v>
+      </c>
+      <c r="G292" t="s">
+        <v>4593</v>
       </c>
     </row>
   </sheetData>

</xml_diff>